<commit_message>
trans excel to xml
</commit_message>
<xml_diff>
--- a/PythonLearning/test.xlsx
+++ b/PythonLearning/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,10 +18,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
-    <t>Passed</t>
+    <t>成功</t>
   </si>
   <si>
-    <t>Failed</t>
+    <t>失败</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
     </row>
     <row r="2" spans="1:600">
       <c r="A2" s="2" t="n">
-        <v>43138.07636140046</v>
+        <v>43260.46307919994</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>

</xml_diff>